<commit_message>
Weekly homework and work on the final project including re-working my data wrangling, working on simulating a dataset from the vegetable portion of my data and re-structuring the data exploration.
</commit_message>
<xml_diff>
--- a/data/tidydata/foodconsumptionRdata.xlsx
+++ b/data/tidydata/foodconsumptionRdata.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffa\OneDrive\Documents\R\Repository\project\tidydata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffa\OneDrive\Documents\R\Repository\data\tidydata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE385D6B-9DBB-4528-BE08-A4D2B3C420DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C040081-7659-463D-824B-702C46623FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A707520-144D-48CE-A482-07B2D71A8EBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A707520-144D-48CE-A482-07B2D71A8EBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Food Consumption By Category" sheetId="1" r:id="rId1"/>
-    <sheet name="Vegetable Fruit and Grain Cons" sheetId="2" r:id="rId2"/>
+    <sheet name="Vegetable Data for Simulation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="57">
   <si>
     <t>lowus</t>
   </si>
@@ -126,143 +126,92 @@
     <t>uphincome</t>
   </si>
   <si>
-    <t xml:space="preserve">   Apples, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Apples as fruit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Apple juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Bananas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Berries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Grapes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Melons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Oranges, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Oranges as fruit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Orange juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Other citrus fruit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Stone fruit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Tropical fruit</t>
-  </si>
-  <si>
-    <t>Vegetables, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Brassica, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Broccoli and cauliflower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Carrots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Celery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Cucumbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Green Peas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Leafy vegetable, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Lettuce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Onions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Peppers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Tomatoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Sweet corn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Potatoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Snap beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Legumes dried</t>
-  </si>
-  <si>
-    <t>Fruit Total</t>
-  </si>
-  <si>
-    <t>Grains, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Corn flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Oat flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Rice dried</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Wheat flour</t>
-  </si>
-  <si>
-    <t>Nuts, Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Peanuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Tree nuts</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>95% CI</t>
-  </si>
-  <si>
-    <t>Pound</t>
-  </si>
-  <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
     <t>07-08</t>
+  </si>
+  <si>
+    <t>meanlb</t>
+  </si>
+  <si>
+    <t>meanloconf</t>
+  </si>
+  <si>
+    <t>meanupconf</t>
+  </si>
+  <si>
+    <t>lowmean</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>leafyveg</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>sweetcorn</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>drylegume</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>brassica</t>
+  </si>
+  <si>
+    <t>brocollicauli</t>
+  </si>
+  <si>
+    <t>carrot</t>
+  </si>
+  <si>
+    <t>celery</t>
+  </si>
+  <si>
+    <t>cucumber</t>
+  </si>
+  <si>
+    <t>greenpea</t>
+  </si>
+  <si>
+    <t>snapbean</t>
+  </si>
+  <si>
+    <t>lowloconf</t>
+  </si>
+  <si>
+    <t>lowupconf</t>
+  </si>
+  <si>
+    <t>highmean</t>
+  </si>
+  <si>
+    <t>highupconf</t>
+  </si>
+  <si>
+    <t>highloconf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +225,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -319,15 +276,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -346,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -354,23 +302,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4922D271-3482-4991-9771-EF98DCE33823}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,8 +649,7 @@
     <col min="5" max="5" width="9.109375" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -749,10 +697,10 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
@@ -2141,7 +2089,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
         <v>20</v>
@@ -2179,7 +2127,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
@@ -2217,7 +2165,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
@@ -2255,7 +2203,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
         <v>20</v>
@@ -2293,7 +2241,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
@@ -2331,7 +2279,7 @@
         <v>15</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
         <v>20</v>
@@ -2369,7 +2317,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
         <v>21</v>
@@ -2407,7 +2355,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
         <v>21</v>
@@ -2445,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -2483,7 +2431,7 @@
         <v>13</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
@@ -2522,7 +2470,7 @@
         <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
@@ -2560,7 +2508,7 @@
         <v>15</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
@@ -2602,10 +2550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF0BA0-5ABF-4BCB-AFC2-6FFDB4FE4139}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,559 +2561,1023 @@
     <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1">
-        <v>108.55</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12">
+        <v>109.8719</v>
+      </c>
+      <c r="D2" s="12">
+        <v>108.2811</v>
+      </c>
+      <c r="E2" s="12">
+        <v>111.47239999999999</v>
+      </c>
+      <c r="F2" s="12">
+        <v>105.69119999999999</v>
+      </c>
+      <c r="G2" s="12">
+        <v>104.2362</v>
+      </c>
+      <c r="H2" s="12">
+        <v>107.14619999999999</v>
+      </c>
+      <c r="I2" s="12">
+        <v>111.76339999999999</v>
+      </c>
+      <c r="J2" s="12">
+        <v>110.10470000000001</v>
+      </c>
+      <c r="K2" s="12">
+        <v>113.4221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
       </c>
       <c r="C3" s="1">
-        <v>107.6</v>
+        <v>6.15</v>
       </c>
       <c r="D3" s="1">
-        <v>109.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.91</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5.68</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.46</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.89</v>
+      </c>
+      <c r="I3" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="J3" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="K3" s="1">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1">
-        <v>24.59</v>
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="1">
-        <v>24.24</v>
+        <v>2.94</v>
       </c>
       <c r="D4" s="1">
-        <v>24.95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.77</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.27</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3.08</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1">
-        <v>13.27</v>
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="1">
-        <v>13.07</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D5" s="1">
-        <v>13.46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.58</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.66</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1">
-        <v>11.11</v>
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>10.83</v>
+        <v>2.12</v>
       </c>
       <c r="D6" s="1">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.88</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.83</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1">
-        <v>10.44</v>
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="1">
-        <v>10.31</v>
+        <v>1.36</v>
       </c>
       <c r="D7" s="1">
-        <v>10.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.31</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1.43</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.37</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.74</v>
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>3.64</v>
+        <v>1.61</v>
       </c>
       <c r="D8" s="1">
-        <v>3.84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.56</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1.77</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.72</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1">
-        <v>6.58</v>
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>6.48</v>
+        <v>0.25</v>
       </c>
       <c r="D9" s="1">
-        <v>6.69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.24</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4.29</v>
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>4.1399999999999997</v>
+        <v>7.42</v>
       </c>
       <c r="D10" s="1">
-        <v>4.4400000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5.18</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8.52</v>
+      </c>
+      <c r="J10" s="1">
+        <v>8.19</v>
+      </c>
+      <c r="K10" s="1">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1">
-        <v>36.35</v>
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="1">
-        <v>35.83</v>
+        <v>4.34</v>
       </c>
       <c r="D11" s="1">
-        <v>36.869999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.22</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.46</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.41</v>
+      </c>
+      <c r="G11" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="I11" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="J11" s="1">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="K11" s="1">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1">
-        <v>3.64</v>
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1">
-        <v>3.55</v>
+        <v>3.31</v>
       </c>
       <c r="D12" s="1">
-        <v>3.73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.52</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3.32</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3.13</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3.52</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3.09</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="1">
-        <v>32.74</v>
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>32.25</v>
+        <v>20.91</v>
       </c>
       <c r="D13" s="1">
-        <v>33.24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20.51</v>
+      </c>
+      <c r="E13" s="1">
+        <v>21.32</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20.66</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20.29</v>
+      </c>
+      <c r="H13" s="1">
+        <v>21.04</v>
+      </c>
+      <c r="I13" s="1">
+        <v>21.02</v>
+      </c>
+      <c r="J13" s="1">
+        <v>20.61</v>
+      </c>
+      <c r="K13" s="1">
+        <v>21.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="1">
-        <v>6.4</v>
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="1">
-        <v>6.18</v>
+        <v>6.53</v>
       </c>
       <c r="D14" s="1">
-        <v>6.61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.35</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6.59</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6.41</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6.77</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>6.32</v>
+      </c>
+      <c r="K14" s="1">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="1">
-        <v>6.37</v>
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>6.24</v>
+        <v>32.326799999999999</v>
       </c>
       <c r="D15" s="1">
-        <v>6.51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31.527000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>33.126599999999996</v>
+      </c>
+      <c r="F15" s="1">
+        <v>33.210300000000004</v>
+      </c>
+      <c r="G15" s="1">
+        <v>32.438400000000001</v>
+      </c>
+      <c r="H15" s="1">
+        <v>33.982199999999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>31.936200000000007</v>
+      </c>
+      <c r="J15" s="1">
+        <v>31.117800000000003</v>
+      </c>
+      <c r="K15" s="1">
+        <v>32.7453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4.3899999999999997</v>
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="1">
-        <v>4.18</v>
+        <v>2.67</v>
       </c>
       <c r="D16" s="1">
-        <v>4.59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.59</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.76</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.78</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.63</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="1">
-        <v>109.8719</v>
+      <c r="B17" t="s">
+        <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>108.2811</v>
+        <v>4.66</v>
       </c>
       <c r="D17" s="1">
-        <v>111.47239999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+        <v>4.51</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6.31</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6.13</v>
+      </c>
+      <c r="H17" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.93</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3.79</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1">
-        <v>6.15</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5.91</v>
-      </c>
-      <c r="D18" s="1">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12">
+        <v>105.72239999999999</v>
+      </c>
+      <c r="D18" s="12">
+        <v>103.6448</v>
+      </c>
+      <c r="E18" s="12">
+        <v>107.80980000000001</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="1">
-        <v>2.94</v>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>2.77</v>
+        <v>6.01</v>
       </c>
       <c r="D19" s="1">
-        <v>3.11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6.32</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="1">
-        <v>4.4000000000000004</v>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="1">
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.8</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="1">
-        <v>2.12</v>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="1">
-        <v>2.0499999999999998</v>
+        <v>3.37</v>
       </c>
       <c r="D21" s="1">
-        <v>2.1800000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.25</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.49</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="1">
-        <v>1.36</v>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="1">
-        <v>1.31</v>
+        <v>1.93</v>
       </c>
       <c r="D22" s="1">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.83</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1">
-        <v>1.61</v>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="1">
+        <v>1.47</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.39</v>
+      </c>
+      <c r="E23" s="1">
         <v>1.56</v>
       </c>
-      <c r="D23" s="1">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="1">
-        <v>0.25</v>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="1">
-        <v>0.24</v>
+        <v>1.39</v>
       </c>
       <c r="D24" s="1">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.34</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8.06</v>
+      </c>
+      <c r="E26" s="1">
+        <v>9.02</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4.67</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3.47</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1">
+        <v>18.829999999999998</v>
+      </c>
+      <c r="D29" s="1">
+        <v>18.23</v>
+      </c>
+      <c r="E29" s="1">
+        <v>19.420000000000002</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5.48</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5.92</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1">
+        <v>31.006200000000003</v>
+      </c>
+      <c r="D31" s="1">
+        <v>29.880900000000004</v>
+      </c>
+      <c r="E31" s="1">
+        <v>32.131499999999996</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1">
-        <v>7.42</v>
-      </c>
-      <c r="C25" s="1">
-        <v>7.15</v>
-      </c>
-      <c r="D25" s="1">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4.34</v>
-      </c>
-      <c r="C26" s="1">
-        <v>4.22</v>
-      </c>
-      <c r="D26" s="1">
-        <v>4.46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="1">
-        <v>3.31</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3.52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1">
-        <v>20.91</v>
-      </c>
-      <c r="C28" s="1">
-        <v>20.51</v>
-      </c>
-      <c r="D28" s="1">
-        <v>21.32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="1">
-        <v>6.53</v>
-      </c>
-      <c r="C29" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="D29" s="1">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="1">
-        <v>32.326799999999999</v>
-      </c>
-      <c r="C30" s="1">
-        <v>31.527000000000001</v>
-      </c>
-      <c r="D30" s="1">
-        <v>33.126599999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.67</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2.59</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4.66</v>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C32" s="1">
-        <v>4.51</v>
+        <v>2.71</v>
       </c>
       <c r="D32" s="1">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.57</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="1">
-        <v>94.76</v>
+        <v>43</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C33" s="1">
-        <v>93.54</v>
+        <v>3.81</v>
       </c>
       <c r="D33" s="1">
-        <v>95.97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.64</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3.98</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="1">
-        <v>9.06</v>
-      </c>
-      <c r="C34" s="1">
-        <v>8.89</v>
-      </c>
-      <c r="D34" s="1">
-        <v>9.23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="1">
-        <v>2.84</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2.81</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="1">
-        <v>8.08</v>
-      </c>
-      <c r="C36" s="1">
-        <v>7.86</v>
-      </c>
-      <c r="D36" s="1">
-        <v>8.31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="1">
-        <v>68.69</v>
-      </c>
-      <c r="C37" s="1">
-        <v>67.62</v>
-      </c>
-      <c r="D37" s="1">
-        <v>69.77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="1">
-        <v>5.67</v>
-      </c>
-      <c r="C38" s="1">
-        <v>5.52</v>
-      </c>
-      <c r="D38" s="1">
-        <v>5.83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="1">
-        <v>4.37</v>
-      </c>
-      <c r="C39" s="1">
-        <v>4.24</v>
-      </c>
-      <c r="D39" s="1">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="11">
-        <v>74.69</v>
-      </c>
-      <c r="C40" s="11">
-        <v>69.66</v>
-      </c>
-      <c r="D40" s="11">
-        <v>79.72</v>
+        <v>49</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>